<commit_message>
enhance vendor management: add image upload functionality and update purchase request handling
</commit_message>
<xml_diff>
--- a/src/productExcelFile.xlsx
+++ b/src/productExcelFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\fastra-frontend\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\web-dev\fastra-frontend\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF38D6A-42A7-460B-9A59-83C433EB70FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD8FAF4-CEDA-48D0-880E-EE496782C33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10155" yWindow="1890" windowWidth="9795" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>product_name</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>total_quantity_purchased</t>
+  </si>
+  <si>
+    <t>consumable</t>
+  </si>
+  <si>
+    <t>service Product</t>
+  </si>
+  <si>
+    <t>stockable</t>
   </si>
 </sst>
 </file>
@@ -369,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:CO5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,9 +392,10 @@
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:93" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,7 +415,35 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="CO2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="CO3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="CO4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="CO5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="You have to select from list" promptTitle="select from list" sqref="C2:C1500" xr:uid="{F9ADFD86-9CBB-4048-96CB-56001338B354}">
+      <formula1>$CO$3:$CO$5</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>